<commit_message>
Drools integrated , bug fix , UI changes ,Json schema bug fix
Drools integrated , bug fix , UI changes ,Json schema bug fix
</commit_message>
<xml_diff>
--- a/openhack-server/src/main/resources/TotalIncome-Gender-DecisionTree.xlsx
+++ b/openhack-server/src/main/resources/TotalIncome-Gender-DecisionTree.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\angular\openhack-devcode-package-master\openhack-server\src\main\resources\com\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CODE BASE\OPENHACK-DEVCODE-PACKAGE\OPENHACK-PORJECT\openhack-server\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D0EF00-3034-4EA8-B3DD-E948ACD12670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +51,6 @@
     <t>ACTION</t>
   </si>
   <si>
-    <t>com.openhack.dev.model.ITR</t>
-  </si>
-  <si>
     <t>Decision table for determining validation messages</t>
   </si>
   <si>
@@ -65,12 +63,6 @@
     <t>Set Validation Messages</t>
   </si>
   <si>
-    <t>$itrObject: ITR</t>
-  </si>
-  <si>
-    <t>$itrObject.partBTI.totalTI &gt; $param</t>
-  </si>
-  <si>
     <t>High Income Assessee</t>
   </si>
   <si>
@@ -84,12 +76,21 @@
   </si>
   <si>
     <t>Assessee has greater than 80K Income</t>
+  </si>
+  <si>
+    <t>$itrObject: RootJosonObject</t>
+  </si>
+  <si>
+    <t>com.openhack.dev.domain.RootJosonObject</t>
+  </si>
+  <si>
+    <t>$itrObject.itr3.partBTI.totalTI &gt; $param</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,21 +501,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,31 +523,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -557,52 +558,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="11">
         <v>50000</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" s="11">
         <v>80000</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>